<commit_message>
feat: update Task_Master_Groups.xlsx for improved data management
</commit_message>
<xml_diff>
--- a/test-data/ConstructIQ/Task_Master _Groups.xlsx
+++ b/test-data/ConstructIQ/Task_Master _Groups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Code/nap-serv/test-data/ConstructIQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62194697-EDC4-AC42-A060-315247A1200F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CE0A08-6A27-484E-BC6A-F88D4F283714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="1000" windowWidth="23360" windowHeight="18640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1000" windowWidth="23360" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_groups" sheetId="1" r:id="rId1"/>
@@ -845,20 +845,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="50.83203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -872,7 +872,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>10</v>
       </c>
       <c r="B2" t="s">
@@ -886,7 +886,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>20</v>
       </c>
       <c r="B3" t="s">
@@ -900,7 +900,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>30</v>
       </c>
       <c r="B4" t="s">
@@ -914,7 +914,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>40</v>
       </c>
       <c r="B5" t="s">
@@ -928,7 +928,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>50</v>
       </c>
       <c r="B6" t="s">
@@ -942,7 +942,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>60</v>
       </c>
       <c r="B7" t="s">
@@ -956,7 +956,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>70</v>
       </c>
       <c r="B8" t="s">
@@ -970,7 +970,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>80</v>
       </c>
       <c r="B9" t="s">
@@ -984,7 +984,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>90</v>
       </c>
       <c r="B10" t="s">
@@ -1006,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+    <sheetView zoomScale="109" workbookViewId="0">
       <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chore: update Task_Master_Groups.xlsx with new data
</commit_message>
<xml_diff>
--- a/test-data/ConstructIQ/Task_Master _Groups.xlsx
+++ b/test-data/ConstructIQ/Task_Master _Groups.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Code/nap-serv/test-data/ConstructIQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CE0A08-6A27-484E-BC6A-F88D4F283714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7522CD83-1D73-2A4F-B7F8-A316D1D2A4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1000" windowWidth="23360" windowHeight="18640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1000" windowWidth="23360" windowHeight="18640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_groups" sheetId="1" r:id="rId1"/>
     <sheet name="task_master" sheetId="2" r:id="rId2"/>
+    <sheet name="template_tasks" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="152">
   <si>
     <t>code</t>
   </si>
@@ -321,9 +322,6 @@
     <t>Appliance Installation</t>
   </si>
   <si>
-    <t>Inspection (Erosion /Tree Protection)</t>
-  </si>
-  <si>
     <t>20.600</t>
   </si>
   <si>
@@ -366,9 +364,6 @@
     <t>60.1100</t>
   </si>
   <si>
-    <t>60.1200</t>
-  </si>
-  <si>
     <t>70.300</t>
   </si>
   <si>
@@ -463,6 +458,39 @@
   </si>
   <si>
     <t>80.500</t>
+  </si>
+  <si>
+    <t>template_id</t>
+  </si>
+  <si>
+    <t>task_code</t>
+  </si>
+  <si>
+    <t>20.500</t>
+  </si>
+  <si>
+    <t>Erosion / Tree Control</t>
+  </si>
+  <si>
+    <t>Inspection (Erosion / Tree Protection)</t>
+  </si>
+  <si>
+    <t>Foundation Walls</t>
+  </si>
+  <si>
+    <t>30.900</t>
+  </si>
+  <si>
+    <t>Siding</t>
+  </si>
+  <si>
+    <t>50.200</t>
+  </si>
+  <si>
+    <t>0197e29a-d4cd-7d3b-b1b1-f65b2bd20220</t>
+  </si>
+  <si>
+    <t>60.800</t>
   </si>
 </sst>
 </file>
@@ -845,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -865,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -879,7 +907,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -893,7 +921,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -907,7 +935,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -921,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -935,7 +963,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -946,10 +974,10 @@
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -963,7 +991,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -977,7 +1005,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -991,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1004,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="A33" sqref="A33:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,10 +1234,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1221,25 +1249,25 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
       </c>
       <c r="E14" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
@@ -1251,10 +1279,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1266,10 +1294,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1281,10 +1309,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" t="b">
         <v>1</v>
@@ -1296,10 +1324,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19" t="b">
         <v>1</v>
@@ -1311,10 +1339,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D20" t="b">
         <v>1</v>
@@ -1326,10 +1354,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>146</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -1341,40 +1369,40 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>33</v>
+        <v>147</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="E23" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
@@ -1386,40 +1414,40 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="E25" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
@@ -1429,12 +1457,12 @@
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>148</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -1446,10 +1474,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>99</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1461,55 +1489,55 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="E30" s="3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
       </c>
       <c r="E31" s="3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
       </c>
       <c r="E32" s="3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
@@ -1521,10 +1549,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
@@ -1536,10 +1564,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -1551,10 +1579,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1566,10 +1594,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -1581,10 +1609,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -1596,10 +1624,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -1611,10 +1639,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1626,55 +1654,55 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
       </c>
       <c r="E41" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
       </c>
       <c r="E42" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
       </c>
       <c r="E43" s="3">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>112</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
@@ -1686,10 +1714,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
@@ -1701,10 +1729,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -1716,10 +1744,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -1731,10 +1759,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>73</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -1746,10 +1774,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -1761,10 +1789,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -1776,10 +1804,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -1791,55 +1819,55 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>39</v>
+        <v>121</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
       </c>
       <c r="E52" s="3">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
       </c>
       <c r="E53" s="3">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>41</v>
+        <v>123</v>
       </c>
       <c r="B54" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
       </c>
       <c r="E54" s="3">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>141</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
@@ -1851,10 +1879,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>142</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
@@ -1862,61 +1890,791 @@
       <c r="E56" s="3">
         <v>80</v>
       </c>
+      <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
       </c>
       <c r="E57" s="3">
-        <v>90</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>43</v>
+        <v>139</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
       </c>
       <c r="E58" s="3">
-        <v>90</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>44</v>
+        <v>140</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>125</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
       </c>
       <c r="E59" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
       </c>
       <c r="E60" s="3">
         <v>90</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" t="s">
+        <v>87</v>
+      </c>
+      <c r="D61" t="b">
+        <v>1</v>
+      </c>
+      <c r="E61" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" t="b">
+        <v>1</v>
+      </c>
+      <c r="E62" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>89</v>
+      </c>
+      <c r="D63" t="b">
+        <v>1</v>
+      </c>
+      <c r="E63" s="3">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3863AB-9EE7-0046-A414-D2A25DA6BACF}">
+  <dimension ref="A1:D60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:B43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>150</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>150</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>150</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>150</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>150</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>150</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>150</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>150</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>150</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>150</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>150</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>150</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>150</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>150</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C51" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>150</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C52" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>150</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>150</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>150</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: update Task_Master_Groups.xlsx by replacing with new data and removing temporary file
</commit_message>
<xml_diff>
--- a/test-data/ConstructIQ/Task_Master _Groups.xlsx
+++ b/test-data/ConstructIQ/Task_Master _Groups.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ian/Code/nap-serv/test-data/ConstructIQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7522CD83-1D73-2A4F-B7F8-A316D1D2A4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FEBF3D2-FBFB-A743-ADBC-234CECFEB068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="1000" windowWidth="23360" windowHeight="18640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="1360" windowWidth="23360" windowHeight="17260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="task_groups" sheetId="1" r:id="rId1"/>
     <sheet name="task_master" sheetId="2" r:id="rId2"/>
     <sheet name="template_tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="template_cost_items" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="233">
   <si>
     <t>code</t>
   </si>
@@ -241,9 +242,6 @@
     <t>Sheathing &amp; Weather Barrier</t>
   </si>
   <si>
-    <t>Exterior Painting &amp; Cladding</t>
-  </si>
-  <si>
     <t>Roofing Installation</t>
   </si>
   <si>
@@ -292,9 +290,6 @@
     <t>Flooring Installation</t>
   </si>
   <si>
-    <t>Cabinetry &amp; Trim</t>
-  </si>
-  <si>
     <t>Inspection (Final MEP Systems)</t>
   </si>
   <si>
@@ -319,9 +314,6 @@
     <t>Fire Sprinkler Installation</t>
   </si>
   <si>
-    <t>Appliance Installation</t>
-  </si>
-  <si>
     <t>20.600</t>
   </si>
   <si>
@@ -481,16 +473,268 @@
     <t>30.900</t>
   </si>
   <si>
-    <t>Siding</t>
-  </si>
-  <si>
     <t>50.200</t>
   </si>
   <si>
-    <t>0197e29a-d4cd-7d3b-b1b1-f65b2bd20220</t>
-  </si>
-  <si>
     <t>60.800</t>
+  </si>
+  <si>
+    <t>is_milestone</t>
+  </si>
+  <si>
+    <t>0197e589-1f28-7eb6-abf9-a5665d0f6bff</t>
+  </si>
+  <si>
+    <t>Trim Soffits and Facia</t>
+  </si>
+  <si>
+    <t>Gutters</t>
+  </si>
+  <si>
+    <t>50.700</t>
+  </si>
+  <si>
+    <t>50.800</t>
+  </si>
+  <si>
+    <t>Appliances</t>
+  </si>
+  <si>
+    <t>Interior Trim</t>
+  </si>
+  <si>
+    <t>Cabinets</t>
+  </si>
+  <si>
+    <t>70.1200</t>
+  </si>
+  <si>
+    <t>Exterior Painting</t>
+  </si>
+  <si>
+    <t>Exterior Cladding</t>
+  </si>
+  <si>
+    <t>unit_name</t>
+  </si>
+  <si>
+    <t>unit_version</t>
+  </si>
+  <si>
+    <t>parent_code</t>
+  </si>
+  <si>
+    <t>cost_class</t>
+  </si>
+  <si>
+    <t>cost_source</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>unit_cost</t>
+  </si>
+  <si>
+    <t>labor</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>turnkey</t>
+  </si>
+  <si>
+    <t>Custom architectural plans and blueprints for the home</t>
+  </si>
+  <si>
+    <t>Structural and MEP (mechanical electrical plumbing) engineering plans</t>
+  </si>
+  <si>
+    <t>Obtaining necessary building permits and approvals</t>
+  </si>
+  <si>
+    <t>Financial planning and loan setup for project funding</t>
+  </si>
+  <si>
+    <t>Creating project timeline and coordination schedule</t>
+  </si>
+  <si>
+    <t>Sourcing long-lead items like windows and doors</t>
+  </si>
+  <si>
+    <t>Initial site inspection for compliance and readiness</t>
+  </si>
+  <si>
+    <t>Land surveying and soil analysis for foundation design</t>
+  </si>
+  <si>
+    <t>Removing vegetation and excavating for foundation</t>
+  </si>
+  <si>
+    <t>Install temporary power water and sanitation</t>
+  </si>
+  <si>
+    <t>Leveling and preparing site for construction</t>
+  </si>
+  <si>
+    <t>Install erosion control measures and tree protection</t>
+  </si>
+  <si>
+    <t>Inspection of erosion and tree protection measures</t>
+  </si>
+  <si>
+    <t>Constructing forms for concrete footings and slab</t>
+  </si>
+  <si>
+    <t>Install reinforcing steel bars for foundation</t>
+  </si>
+  <si>
+    <t>Inspection of footings before concrete pour</t>
+  </si>
+  <si>
+    <t>Install underground plumbing for drainage and supply</t>
+  </si>
+  <si>
+    <t>Inspection of underground plumbing installation</t>
+  </si>
+  <si>
+    <t>Pouring concrete for footings and slab foundation</t>
+  </si>
+  <si>
+    <t>Constructing concrete foundation walls</t>
+  </si>
+  <si>
+    <t>Applying waterproofing to foundation walls</t>
+  </si>
+  <si>
+    <t>Inspection of slab after pouring</t>
+  </si>
+  <si>
+    <t>Constructing wall and floor framing with lumber</t>
+  </si>
+  <si>
+    <t>Constructing roof trusses and framing</t>
+  </si>
+  <si>
+    <t>Inspection of framing for structural integrity</t>
+  </si>
+  <si>
+    <t>Install exterior sheathing and weather-resistant barrier</t>
+  </si>
+  <si>
+    <t>Install mid-range windows</t>
+  </si>
+  <si>
+    <t>Install asphalt shingle roofing</t>
+  </si>
+  <si>
+    <t>Inspection of roof sheathing installation</t>
+  </si>
+  <si>
+    <t>Install exterior trim</t>
+  </si>
+  <si>
+    <t>Install fiber cement siding on exterior walls</t>
+  </si>
+  <si>
+    <t>Install gutters</t>
+  </si>
+  <si>
+    <t>Paint home exterior</t>
+  </si>
+  <si>
+    <t>Install rough-in plumbing pipes and vents</t>
+  </si>
+  <si>
+    <t>Inspection of rough-in plumbing</t>
+  </si>
+  <si>
+    <t>Install electrical wiring and boxes</t>
+  </si>
+  <si>
+    <t>Inspection of rough-in electrical</t>
+  </si>
+  <si>
+    <t>Install HVAC ductwork and rough-in components</t>
+  </si>
+  <si>
+    <t>Inspection of HVAC rough-in</t>
+  </si>
+  <si>
+    <t>Install fire sprinkler system</t>
+  </si>
+  <si>
+    <t>Install fiberglass batt insulation</t>
+  </si>
+  <si>
+    <t>Inspection of insulation installation</t>
+  </si>
+  <si>
+    <t>Install and taping drywall</t>
+  </si>
+  <si>
+    <t>Inspection for energy code compliance</t>
+  </si>
+  <si>
+    <t>Applying interior paint to walls and ceilings</t>
+  </si>
+  <si>
+    <t>Install mid-range flooring (e.g. hardwood tile)</t>
+  </si>
+  <si>
+    <t>Install  interior trim</t>
+  </si>
+  <si>
+    <t>Kitchen Cabinets</t>
+  </si>
+  <si>
+    <t>Install kitchen and laundry appliances</t>
+  </si>
+  <si>
+    <t>Install sinks faucets and toilets</t>
+  </si>
+  <si>
+    <t>Install lighting and electrical fixtures</t>
+  </si>
+  <si>
+    <t>Install HVAC units and final components</t>
+  </si>
+  <si>
+    <t>Initial cleanup after rough-in phases</t>
+  </si>
+  <si>
+    <t>Touching up drywall imperfections</t>
+  </si>
+  <si>
+    <t>Touching up interior paint</t>
+  </si>
+  <si>
+    <t>Final cleanup before occupancy</t>
+  </si>
+  <si>
+    <t>Install sod plants and basic landscaping</t>
+  </si>
+  <si>
+    <t>Install concrete driveway</t>
+  </si>
+  <si>
+    <t>Final inspection of MEP systems</t>
+  </si>
+  <si>
+    <t>Final building inspection</t>
+  </si>
+  <si>
+    <t>Final site and grading inspection</t>
+  </si>
+  <si>
+    <t>Inspection for certificate of occupancy</t>
+  </si>
+  <si>
+    <t>Tempest</t>
+  </si>
+  <si>
+    <t>item_code</t>
   </si>
 </sst>
 </file>
@@ -893,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -907,7 +1151,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -921,7 +1165,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -935,7 +1179,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -949,7 +1193,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -963,7 +1207,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D6">
         <v>5</v>
@@ -974,10 +1218,10 @@
         <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D7">
         <v>6</v>
@@ -991,7 +1235,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -1005,7 +1249,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -1019,7 +1263,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D10">
         <v>9</v>
@@ -1032,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A43"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1045,9 +1289,9 @@
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -1058,13 +1302,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1080,7 +1327,9 @@
       <c r="E2" s="3">
         <v>10</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -1095,7 +1344,9 @@
       <c r="E3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1110,7 +1361,9 @@
       <c r="E4" s="3">
         <v>10</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1125,7 +1378,9 @@
       <c r="E5" s="3">
         <v>10</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
@@ -1140,7 +1395,9 @@
       <c r="E6" s="3">
         <v>10</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -1155,7 +1412,9 @@
       <c r="E7" s="3">
         <v>10</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -1170,7 +1429,9 @@
       <c r="E8" s="3">
         <v>10</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -1185,7 +1446,9 @@
       <c r="E9" s="3">
         <v>20</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -1200,7 +1463,9 @@
       <c r="E10" s="3">
         <v>20</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -1215,7 +1480,9 @@
       <c r="E11" s="3">
         <v>20</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
@@ -1230,14 +1497,16 @@
       <c r="E12" s="3">
         <v>20</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1245,14 +1514,16 @@
       <c r="E13" s="3">
         <v>20</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D14" t="b">
         <v>1</v>
@@ -1260,7 +1531,9 @@
       <c r="E14" s="3">
         <v>20</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
@@ -1275,7 +1548,9 @@
       <c r="E15" s="3">
         <v>30</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
@@ -1290,7 +1565,9 @@
       <c r="E16" s="3">
         <v>30</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -1305,7 +1582,9 @@
       <c r="E17" s="3">
         <v>30</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
@@ -1320,7 +1599,9 @@
       <c r="E18" s="3">
         <v>30</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
@@ -1335,7 +1616,9 @@
       <c r="E19" s="3">
         <v>30</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -1350,14 +1633,16 @@
       <c r="E20" s="3">
         <v>30</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D21" t="b">
         <v>1</v>
@@ -1365,7 +1650,9 @@
       <c r="E21" s="3">
         <v>30</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -1380,11 +1667,13 @@
       <c r="E22" s="3">
         <v>30</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B23" t="s">
         <v>63</v>
@@ -1395,7 +1684,9 @@
       <c r="E23" s="3">
         <v>30</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -1410,7 +1701,9 @@
       <c r="E24" s="3">
         <v>40</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -1425,7 +1718,9 @@
       <c r="E25" s="3">
         <v>40</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
@@ -1440,7 +1735,9 @@
       <c r="E26" s="3">
         <v>40</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -1455,14 +1752,16 @@
       <c r="E27" s="3">
         <v>50</v>
       </c>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B28" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
@@ -1470,14 +1769,16 @@
       <c r="E28" s="3">
         <v>50</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1485,11 +1786,13 @@
       <c r="E29" s="3">
         <v>50</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
         <v>69</v>
@@ -1500,14 +1803,16 @@
       <c r="E30" s="3">
         <v>50</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="D31" t="b">
         <v>1</v>
@@ -1515,14 +1820,16 @@
       <c r="E31" s="3">
         <v>50</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="D32" t="b">
         <v>1</v>
@@ -1530,44 +1837,50 @@
       <c r="E32" s="3">
         <v>50</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="D33" t="b">
         <v>1</v>
       </c>
       <c r="E33" s="3">
-        <v>60</v>
-      </c>
-      <c r="F33" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="F33" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="E34" s="3">
-        <v>60</v>
-      </c>
-      <c r="F34" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="F34" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
@@ -1575,14 +1888,16 @@
       <c r="E35" s="3">
         <v>60</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
@@ -1590,14 +1905,16 @@
       <c r="E36" s="3">
         <v>60</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D37" t="b">
         <v>1</v>
@@ -1605,14 +1922,16 @@
       <c r="E37" s="3">
         <v>60</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
@@ -1620,14 +1939,16 @@
       <c r="E38" s="3">
         <v>60</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
@@ -1635,14 +1956,16 @@
       <c r="E39" s="3">
         <v>60</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D40" t="b">
         <v>1</v>
@@ -1650,14 +1973,16 @@
       <c r="E40" s="3">
         <v>60</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="D41" t="b">
         <v>1</v>
@@ -1665,14 +1990,16 @@
       <c r="E41" s="3">
         <v>60</v>
       </c>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D42" t="b">
         <v>1</v>
@@ -1680,14 +2007,16 @@
       <c r="E42" s="3">
         <v>60</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
@@ -1695,44 +2024,50 @@
       <c r="E43" s="3">
         <v>60</v>
       </c>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D44" t="b">
         <v>1</v>
       </c>
       <c r="E44" s="3">
-        <v>70</v>
-      </c>
-      <c r="F44" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="F44" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D45" t="b">
         <v>1</v>
       </c>
       <c r="E45" s="3">
-        <v>70</v>
-      </c>
-      <c r="F45" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="F45" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
@@ -1740,14 +2075,16 @@
       <c r="E46" s="3">
         <v>70</v>
       </c>
-      <c r="F46" s="3"/>
+      <c r="F46" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
@@ -1755,14 +2092,16 @@
       <c r="E47" s="3">
         <v>70</v>
       </c>
-      <c r="F47" s="3"/>
+      <c r="F47" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
@@ -1770,14 +2109,16 @@
       <c r="E48" s="3">
         <v>70</v>
       </c>
-      <c r="F48" s="3"/>
+      <c r="F48" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
       <c r="D49" t="b">
         <v>1</v>
@@ -1785,14 +2126,16 @@
       <c r="E49" s="3">
         <v>70</v>
       </c>
-      <c r="F49" s="3"/>
+      <c r="F49" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
@@ -1800,14 +2143,16 @@
       <c r="E50" s="3">
         <v>70</v>
       </c>
-      <c r="F50" s="3"/>
+      <c r="F50" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="D51" t="b">
         <v>1</v>
@@ -1815,14 +2160,16 @@
       <c r="E51" s="3">
         <v>70</v>
       </c>
-      <c r="F51" s="3"/>
+      <c r="F51" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B52" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
       <c r="D52" t="b">
         <v>1</v>
@@ -1830,14 +2177,16 @@
       <c r="E52" s="3">
         <v>70</v>
       </c>
-      <c r="F52" s="3"/>
+      <c r="F52" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B53" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
@@ -1845,14 +2194,16 @@
       <c r="E53" s="3">
         <v>70</v>
       </c>
-      <c r="F53" s="3"/>
+      <c r="F53" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B54" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D54" t="b">
         <v>1</v>
@@ -1860,59 +2211,67 @@
       <c r="E54" s="3">
         <v>70</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="D55" t="b">
         <v>1</v>
       </c>
       <c r="E55" s="3">
-        <v>80</v>
-      </c>
-      <c r="F55" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="F55" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="D56" t="b">
         <v>1</v>
       </c>
       <c r="E56" s="3">
-        <v>80</v>
-      </c>
-      <c r="F56" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="F56" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>41</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
       </c>
       <c r="E57" s="3">
-        <v>80</v>
-      </c>
-      <c r="F57" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="F57" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="B58" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="D58" t="b">
         <v>1</v>
@@ -1920,14 +2279,16 @@
       <c r="E58" s="3">
         <v>80</v>
       </c>
-      <c r="F58" s="3"/>
+      <c r="F58" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>140</v>
+        <v>40</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D59" t="b">
         <v>1</v>
@@ -1935,61 +2296,127 @@
       <c r="E59" s="3">
         <v>80</v>
       </c>
+      <c r="F59" s="3" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>133</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
       </c>
       <c r="E60" s="3">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="F60" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>43</v>
+        <v>136</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
       </c>
       <c r="E61" s="3">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="F61" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D62" t="b">
         <v>1</v>
       </c>
       <c r="E62" s="3">
-        <v>90</v>
+        <v>80</v>
+      </c>
+      <c r="F62" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
       </c>
       <c r="E63" s="3">
         <v>90</v>
+      </c>
+      <c r="F63" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B64" t="s">
+        <v>85</v>
+      </c>
+      <c r="D64" t="b">
+        <v>1</v>
+      </c>
+      <c r="E64" s="3">
+        <v>90</v>
+      </c>
+      <c r="F64" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D65" t="b">
+        <v>1</v>
+      </c>
+      <c r="E65" s="3">
+        <v>90</v>
+      </c>
+      <c r="F65" s="3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" t="s">
+        <v>87</v>
+      </c>
+      <c r="D66" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" s="3">
+        <v>90</v>
+      </c>
+      <c r="F66" s="3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2000,11 +2427,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3863AB-9EE7-0046-A414-D2A25DA6BACF}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:B43"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2016,21 +2441,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>13</v>
@@ -2041,7 +2466,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>14</v>
@@ -2052,7 +2477,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>15</v>
@@ -2063,7 +2488,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -2074,7 +2499,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
@@ -2085,7 +2510,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -2096,7 +2521,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>19</v>
@@ -2107,7 +2532,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>20</v>
@@ -2118,7 +2543,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
@@ -2129,7 +2554,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>22</v>
@@ -2140,7 +2565,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>23</v>
@@ -2151,29 +2576,29 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C14" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>24</v>
@@ -2184,7 +2609,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>25</v>
@@ -2195,7 +2620,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>26</v>
@@ -2206,7 +2631,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>27</v>
@@ -2217,7 +2642,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>28</v>
@@ -2228,7 +2653,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>29</v>
@@ -2239,18 +2664,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>31</v>
@@ -2261,10 +2686,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C23" t="s">
         <v>63</v>
@@ -2272,7 +2697,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>32</v>
@@ -2283,7 +2708,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>33</v>
@@ -2294,7 +2719,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>34</v>
@@ -2305,7 +2730,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>35</v>
@@ -2316,32 +2741,32 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>148</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
         <v>69</v>
@@ -2349,336 +2774,2975 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" t="s">
         <v>150</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>151</v>
+        <v>100</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>37</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="C45" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="C46" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>110</v>
+        <v>38</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C49" t="s">
-        <v>76</v>
+        <v>155</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C53" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C54" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="C55" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="C56" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="C59" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="C60" t="s">
-        <v>89</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>148</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>148</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C63" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{369E62B8-CBBF-A740-BB78-0002F94E1808}">
+  <dimension ref="A1:J99"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>24500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H3" t="s">
+        <v>170</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>17500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H7" t="s">
+        <v>174</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>166</v>
+      </c>
+      <c r="G9" t="s">
+        <v>168</v>
+      </c>
+      <c r="H9" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" t="s">
+        <v>177</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" t="s">
+        <v>177</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12" t="s">
+        <v>168</v>
+      </c>
+      <c r="H12" t="s">
+        <v>178</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G13" t="s">
+        <v>168</v>
+      </c>
+      <c r="H13" t="s">
+        <v>178</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14" t="s">
+        <v>168</v>
+      </c>
+      <c r="H14" t="s">
+        <v>179</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>231</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>166</v>
+      </c>
+      <c r="G15" t="s">
+        <v>168</v>
+      </c>
+      <c r="H15" t="s">
+        <v>179</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>140</v>
+      </c>
+      <c r="F16" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H16" t="s">
+        <v>180</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" t="s">
+        <v>166</v>
+      </c>
+      <c r="G17" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" t="s">
+        <v>180</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18" t="s">
+        <v>168</v>
+      </c>
+      <c r="H18" t="s">
+        <v>181</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" t="s">
+        <v>167</v>
+      </c>
+      <c r="G19" t="s">
+        <v>168</v>
+      </c>
+      <c r="H19" t="s">
+        <v>182</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>231</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" t="s">
+        <v>168</v>
+      </c>
+      <c r="H20" t="s">
+        <v>182</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>231</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" t="s">
+        <v>183</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>231</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>166</v>
+      </c>
+      <c r="G22" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" t="s">
+        <v>183</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>231</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H23" t="s">
+        <v>184</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F24" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" t="s">
+        <v>168</v>
+      </c>
+      <c r="H24" t="s">
+        <v>185</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" t="s">
+        <v>166</v>
+      </c>
+      <c r="G25" t="s">
+        <v>168</v>
+      </c>
+      <c r="H25" t="s">
+        <v>185</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>231</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" t="s">
+        <v>168</v>
+      </c>
+      <c r="H26" t="s">
+        <v>186</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>231</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" t="s">
+        <v>167</v>
+      </c>
+      <c r="G27" t="s">
+        <v>168</v>
+      </c>
+      <c r="H27" t="s">
+        <v>187</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>7920</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>231</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" t="s">
+        <v>166</v>
+      </c>
+      <c r="G28" t="s">
+        <v>168</v>
+      </c>
+      <c r="H28" t="s">
+        <v>187</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>5280</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>231</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
+        <v>167</v>
+      </c>
+      <c r="G29" t="s">
+        <v>168</v>
+      </c>
+      <c r="H29" t="s">
+        <v>188</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>166</v>
+      </c>
+      <c r="G30" t="s">
+        <v>168</v>
+      </c>
+      <c r="H30" t="s">
+        <v>188</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>231</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H31" t="s">
+        <v>189</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" t="s">
+        <v>166</v>
+      </c>
+      <c r="G32" t="s">
+        <v>168</v>
+      </c>
+      <c r="H32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>2970</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>231</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+      <c r="F33" t="s">
+        <v>166</v>
+      </c>
+      <c r="G33" t="s">
+        <v>168</v>
+      </c>
+      <c r="H33" t="s">
+        <v>190</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" t="s">
+        <v>191</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>231</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="F35" t="s">
+        <v>166</v>
+      </c>
+      <c r="G35" t="s">
+        <v>168</v>
+      </c>
+      <c r="H35" t="s">
+        <v>191</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>231</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
+        <v>168</v>
+      </c>
+      <c r="H36" t="s">
+        <v>192</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>231</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" t="s">
+        <v>168</v>
+      </c>
+      <c r="H37" t="s">
+        <v>192</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="J37">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F38" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" t="s">
+        <v>168</v>
+      </c>
+      <c r="H38" t="s">
+        <v>193</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>231</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" t="s">
+        <v>168</v>
+      </c>
+      <c r="H39" t="s">
+        <v>194</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>35</v>
+      </c>
+      <c r="F40" t="s">
+        <v>166</v>
+      </c>
+      <c r="G40" t="s">
+        <v>168</v>
+      </c>
+      <c r="H40" t="s">
+        <v>194</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>231</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>145</v>
+      </c>
+      <c r="F41" t="s">
+        <v>167</v>
+      </c>
+      <c r="G41" t="s">
+        <v>168</v>
+      </c>
+      <c r="H41" t="s">
+        <v>195</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>231</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>145</v>
+      </c>
+      <c r="F42" t="s">
+        <v>166</v>
+      </c>
+      <c r="G42" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" t="s">
+        <v>195</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>231</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" t="s">
+        <v>167</v>
+      </c>
+      <c r="G43" t="s">
+        <v>168</v>
+      </c>
+      <c r="H43" t="s">
+        <v>196</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>231</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" t="s">
+        <v>166</v>
+      </c>
+      <c r="G44" t="s">
+        <v>168</v>
+      </c>
+      <c r="H44" t="s">
+        <v>196</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>4950</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>231</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" t="s">
+        <v>166</v>
+      </c>
+      <c r="G45" t="s">
+        <v>168</v>
+      </c>
+      <c r="H45" t="s">
+        <v>197</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>231</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" t="s">
+        <v>167</v>
+      </c>
+      <c r="G46" t="s">
+        <v>168</v>
+      </c>
+      <c r="H46" t="s">
+        <v>198</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="J46">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>231</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>94</v>
+      </c>
+      <c r="F47" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" t="s">
+        <v>168</v>
+      </c>
+      <c r="H47" t="s">
+        <v>198</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>231</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+      <c r="F48" t="s">
+        <v>167</v>
+      </c>
+      <c r="G48" t="s">
+        <v>168</v>
+      </c>
+      <c r="H48" t="s">
+        <v>199</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>231</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F49" t="s">
+        <v>166</v>
+      </c>
+      <c r="G49" t="s">
+        <v>168</v>
+      </c>
+      <c r="H49" t="s">
+        <v>199</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>5500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>231</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>151</v>
+      </c>
+      <c r="F50" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50" t="s">
+        <v>168</v>
+      </c>
+      <c r="H50" t="s">
+        <v>200</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>231</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="F51" t="s">
+        <v>166</v>
+      </c>
+      <c r="G51" t="s">
+        <v>168</v>
+      </c>
+      <c r="H51" t="s">
+        <v>200</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>231</v>
+      </c>
+      <c r="B52">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+      <c r="F52" t="s">
+        <v>167</v>
+      </c>
+      <c r="G52" t="s">
+        <v>168</v>
+      </c>
+      <c r="H52" t="s">
+        <v>201</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="J52">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>231</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" t="s">
+        <v>166</v>
+      </c>
+      <c r="G53" t="s">
+        <v>168</v>
+      </c>
+      <c r="H53" t="s">
+        <v>201</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>231</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>89</v>
+      </c>
+      <c r="F54" t="s">
+        <v>167</v>
+      </c>
+      <c r="G54" t="s">
+        <v>168</v>
+      </c>
+      <c r="H54" t="s">
+        <v>202</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="J54">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55" t="s">
+        <v>89</v>
+      </c>
+      <c r="F55" t="s">
+        <v>166</v>
+      </c>
+      <c r="G55" t="s">
+        <v>168</v>
+      </c>
+      <c r="H55" t="s">
+        <v>202</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="J55">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>231</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" t="s">
+        <v>166</v>
+      </c>
+      <c r="G56" t="s">
+        <v>168</v>
+      </c>
+      <c r="H56" t="s">
+        <v>203</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>231</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57" t="s">
+        <v>97</v>
+      </c>
+      <c r="F57" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" t="s">
+        <v>168</v>
+      </c>
+      <c r="H57" t="s">
+        <v>204</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>231</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F58" t="s">
+        <v>166</v>
+      </c>
+      <c r="G58" t="s">
+        <v>168</v>
+      </c>
+      <c r="H58" t="s">
+        <v>204</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G59" t="s">
+        <v>168</v>
+      </c>
+      <c r="H59" t="s">
+        <v>205</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>231</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>99</v>
+      </c>
+      <c r="F60" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" t="s">
+        <v>168</v>
+      </c>
+      <c r="H60" t="s">
+        <v>206</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>231</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" t="s">
+        <v>166</v>
+      </c>
+      <c r="G61" t="s">
+        <v>168</v>
+      </c>
+      <c r="H61" t="s">
+        <v>206</v>
+      </c>
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>231</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>100</v>
+      </c>
+      <c r="F62" t="s">
+        <v>166</v>
+      </c>
+      <c r="G62" t="s">
+        <v>168</v>
+      </c>
+      <c r="H62" t="s">
+        <v>207</v>
+      </c>
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>231</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" t="s">
+        <v>101</v>
+      </c>
+      <c r="F63" t="s">
+        <v>167</v>
+      </c>
+      <c r="G63" t="s">
+        <v>168</v>
+      </c>
+      <c r="H63" t="s">
+        <v>208</v>
+      </c>
+      <c r="I63">
+        <v>1</v>
+      </c>
+      <c r="J63">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>231</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>101</v>
+      </c>
+      <c r="F64" t="s">
+        <v>166</v>
+      </c>
+      <c r="G64" t="s">
+        <v>168</v>
+      </c>
+      <c r="H64" t="s">
+        <v>208</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>231</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>146</v>
+      </c>
+      <c r="F65" t="s">
+        <v>167</v>
+      </c>
+      <c r="G65" t="s">
+        <v>168</v>
+      </c>
+      <c r="H65" t="s">
+        <v>209</v>
+      </c>
+      <c r="I65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>231</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>146</v>
+      </c>
+      <c r="F66" t="s">
+        <v>166</v>
+      </c>
+      <c r="G66" t="s">
+        <v>168</v>
+      </c>
+      <c r="H66" t="s">
+        <v>209</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>231</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67" t="s">
+        <v>103</v>
+      </c>
+      <c r="F67" t="s">
+        <v>166</v>
+      </c>
+      <c r="G67" t="s">
+        <v>168</v>
+      </c>
+      <c r="H67" t="s">
+        <v>210</v>
+      </c>
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>231</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68" t="s">
+        <v>89</v>
+      </c>
+      <c r="F68" t="s">
+        <v>167</v>
+      </c>
+      <c r="G68" t="s">
+        <v>168</v>
+      </c>
+      <c r="H68" t="s">
+        <v>211</v>
+      </c>
+      <c r="I68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>231</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>89</v>
+      </c>
+      <c r="F69" t="s">
+        <v>166</v>
+      </c>
+      <c r="G69" t="s">
+        <v>168</v>
+      </c>
+      <c r="H69" t="s">
+        <v>211</v>
+      </c>
+      <c r="I69">
+        <v>1</v>
+      </c>
+      <c r="J69">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>105</v>
+      </c>
+      <c r="F70" t="s">
+        <v>166</v>
+      </c>
+      <c r="G70" t="s">
+        <v>168</v>
+      </c>
+      <c r="H70" t="s">
+        <v>212</v>
+      </c>
+      <c r="I70">
+        <v>1</v>
+      </c>
+      <c r="J70">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>231</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>37</v>
+      </c>
+      <c r="F71" t="s">
+        <v>167</v>
+      </c>
+      <c r="G71" t="s">
+        <v>168</v>
+      </c>
+      <c r="H71" t="s">
+        <v>213</v>
+      </c>
+      <c r="I71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>231</v>
+      </c>
+      <c r="B72">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>37</v>
+      </c>
+      <c r="F72" t="s">
+        <v>166</v>
+      </c>
+      <c r="G72" t="s">
+        <v>168</v>
+      </c>
+      <c r="H72" t="s">
+        <v>213</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+      <c r="J72">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>231</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>38</v>
+      </c>
+      <c r="F73" t="s">
+        <v>167</v>
+      </c>
+      <c r="G73" t="s">
+        <v>168</v>
+      </c>
+      <c r="H73" t="s">
+        <v>214</v>
+      </c>
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>231</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="F74" t="s">
+        <v>166</v>
+      </c>
+      <c r="G74" t="s">
+        <v>168</v>
+      </c>
+      <c r="H74" t="s">
+        <v>214</v>
+      </c>
+      <c r="I74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>231</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>106</v>
+      </c>
+      <c r="F75" t="s">
+        <v>167</v>
+      </c>
+      <c r="G75" t="s">
+        <v>168</v>
+      </c>
+      <c r="H75" t="s">
+        <v>215</v>
+      </c>
+      <c r="I75">
+        <v>1</v>
+      </c>
+      <c r="J75">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>231</v>
+      </c>
+      <c r="B76">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>106</v>
+      </c>
+      <c r="F76" t="s">
+        <v>166</v>
+      </c>
+      <c r="G76" t="s">
+        <v>168</v>
+      </c>
+      <c r="H76" t="s">
+        <v>215</v>
+      </c>
+      <c r="I76">
+        <v>1</v>
+      </c>
+      <c r="J76">
+        <v>4800</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>231</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>107</v>
+      </c>
+      <c r="F77" t="s">
+        <v>167</v>
+      </c>
+      <c r="G77" t="s">
+        <v>168</v>
+      </c>
+      <c r="H77" t="s">
+        <v>216</v>
+      </c>
+      <c r="I77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>231</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>114</v>
+      </c>
+      <c r="F78" t="s">
+        <v>167</v>
+      </c>
+      <c r="G78" t="s">
+        <v>168</v>
+      </c>
+      <c r="H78" t="s">
+        <v>217</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>6400</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>231</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>114</v>
+      </c>
+      <c r="F79" t="s">
+        <v>166</v>
+      </c>
+      <c r="G79" t="s">
+        <v>168</v>
+      </c>
+      <c r="H79" t="s">
+        <v>217</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>231</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>115</v>
+      </c>
+      <c r="F80" t="s">
+        <v>167</v>
+      </c>
+      <c r="G80" t="s">
+        <v>168</v>
+      </c>
+      <c r="H80" t="s">
+        <v>218</v>
+      </c>
+      <c r="I80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>231</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81" t="s">
+        <v>115</v>
+      </c>
+      <c r="F81" t="s">
+        <v>166</v>
+      </c>
+      <c r="G81" t="s">
+        <v>168</v>
+      </c>
+      <c r="H81" t="s">
+        <v>218</v>
+      </c>
+      <c r="I81">
+        <v>1</v>
+      </c>
+      <c r="J81">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>231</v>
+      </c>
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>116</v>
+      </c>
+      <c r="F82" t="s">
+        <v>167</v>
+      </c>
+      <c r="G82" t="s">
+        <v>168</v>
+      </c>
+      <c r="H82" t="s">
+        <v>219</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+      <c r="J82">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>231</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>116</v>
+      </c>
+      <c r="F83" t="s">
+        <v>166</v>
+      </c>
+      <c r="G83" t="s">
+        <v>168</v>
+      </c>
+      <c r="H83" t="s">
+        <v>219</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>231</v>
+      </c>
+      <c r="B84">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>117</v>
+      </c>
+      <c r="F84" t="s">
+        <v>167</v>
+      </c>
+      <c r="G84" t="s">
+        <v>168</v>
+      </c>
+      <c r="H84" t="s">
+        <v>220</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>231</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>117</v>
+      </c>
+      <c r="F85" t="s">
+        <v>166</v>
+      </c>
+      <c r="G85" t="s">
+        <v>168</v>
+      </c>
+      <c r="H85" t="s">
+        <v>220</v>
+      </c>
+      <c r="I85">
+        <v>1</v>
+      </c>
+      <c r="J85">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>231</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>118</v>
+      </c>
+      <c r="F86" t="s">
+        <v>166</v>
+      </c>
+      <c r="G86" t="s">
+        <v>168</v>
+      </c>
+      <c r="H86" t="s">
+        <v>221</v>
+      </c>
+      <c r="I86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>231</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>37</v>
+      </c>
+      <c r="F87" t="s">
+        <v>167</v>
+      </c>
+      <c r="G87" t="s">
+        <v>168</v>
+      </c>
+      <c r="H87" t="s">
+        <v>222</v>
+      </c>
+      <c r="I87">
+        <v>1</v>
+      </c>
+      <c r="J87">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>231</v>
+      </c>
+      <c r="B88">
+        <v>1</v>
+      </c>
+      <c r="C88" t="s">
+        <v>37</v>
+      </c>
+      <c r="F88" t="s">
+        <v>166</v>
+      </c>
+      <c r="G88" t="s">
+        <v>168</v>
+      </c>
+      <c r="H88" t="s">
+        <v>222</v>
+      </c>
+      <c r="I88">
+        <v>1</v>
+      </c>
+      <c r="J88">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>231</v>
+      </c>
+      <c r="B89">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>120</v>
+      </c>
+      <c r="F89" t="s">
+        <v>167</v>
+      </c>
+      <c r="G89" t="s">
+        <v>168</v>
+      </c>
+      <c r="H89" t="s">
+        <v>223</v>
+      </c>
+      <c r="I89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>231</v>
+      </c>
+      <c r="B90">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>120</v>
+      </c>
+      <c r="F90" t="s">
+        <v>166</v>
+      </c>
+      <c r="G90" t="s">
+        <v>168</v>
+      </c>
+      <c r="H90" t="s">
+        <v>223</v>
+      </c>
+      <c r="I90">
+        <v>1</v>
+      </c>
+      <c r="J90">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>231</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91" t="s">
+        <v>156</v>
+      </c>
+      <c r="F91" t="s">
+        <v>166</v>
+      </c>
+      <c r="G91" t="s">
+        <v>168</v>
+      </c>
+      <c r="H91" t="s">
+        <v>224</v>
+      </c>
+      <c r="I91">
+        <v>1</v>
+      </c>
+      <c r="J91">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>231</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>39</v>
+      </c>
+      <c r="F92" t="s">
+        <v>167</v>
+      </c>
+      <c r="G92" t="s">
+        <v>168</v>
+      </c>
+      <c r="H92" t="s">
+        <v>225</v>
+      </c>
+      <c r="I92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>231</v>
+      </c>
+      <c r="B93">
+        <v>1</v>
+      </c>
+      <c r="C93" t="s">
+        <v>39</v>
+      </c>
+      <c r="F93" t="s">
+        <v>166</v>
+      </c>
+      <c r="G93" t="s">
+        <v>168</v>
+      </c>
+      <c r="H93" t="s">
+        <v>225</v>
+      </c>
+      <c r="I93">
+        <v>1</v>
+      </c>
+      <c r="J93">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>231</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+      <c r="C94" t="s">
+        <v>137</v>
+      </c>
+      <c r="F94" t="s">
+        <v>167</v>
+      </c>
+      <c r="G94" t="s">
+        <v>168</v>
+      </c>
+      <c r="H94" t="s">
+        <v>226</v>
+      </c>
+      <c r="I94">
+        <v>1</v>
+      </c>
+      <c r="J94">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>231</v>
+      </c>
+      <c r="B95">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>137</v>
+      </c>
+      <c r="F95" t="s">
+        <v>166</v>
+      </c>
+      <c r="G95" t="s">
+        <v>168</v>
+      </c>
+      <c r="H95" t="s">
+        <v>226</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>231</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96" t="s">
+        <v>42</v>
+      </c>
+      <c r="F96" t="s">
+        <v>166</v>
+      </c>
+      <c r="G96" t="s">
+        <v>168</v>
+      </c>
+      <c r="H96" t="s">
+        <v>227</v>
+      </c>
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="J96">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>231</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>43</v>
+      </c>
+      <c r="F97" t="s">
+        <v>166</v>
+      </c>
+      <c r="G97" t="s">
+        <v>168</v>
+      </c>
+      <c r="H97" t="s">
+        <v>228</v>
+      </c>
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>231</v>
+      </c>
+      <c r="B98">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>44</v>
+      </c>
+      <c r="F98" t="s">
+        <v>166</v>
+      </c>
+      <c r="G98" t="s">
+        <v>168</v>
+      </c>
+      <c r="H98" t="s">
+        <v>229</v>
+      </c>
+      <c r="I98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>231</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>108</v>
+      </c>
+      <c r="F99" t="s">
+        <v>166</v>
+      </c>
+      <c r="G99" t="s">
+        <v>168</v>
+      </c>
+      <c r="H99" t="s">
+        <v>230</v>
+      </c>
+      <c r="I99">
+        <v>1</v>
+      </c>
+      <c r="J99">
+        <v>500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>